<commit_message>
muestra datos de exel en un treeview
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenin\PycharmProjects\aceptconcret\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79C1F34-F56F-48CD-827C-775A65D23AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBB9F1C-6DA5-448F-9E79-12715B25AE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7875" xr2:uid="{1081E678-B354-4679-BACA-BA65C3BB3F83}"/>
+    <workbookView xWindow="-15300" yWindow="600" windowWidth="14550" windowHeight="12225" xr2:uid="{1081E678-B354-4679-BACA-BA65C3BB3F83}"/>
   </bookViews>
   <sheets>
     <sheet name="Libro1" sheetId="1" r:id="rId1"/>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C455D7-37C5-499A-9B3A-C9F5DF937DE6}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,115 +418,446 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>44562</v>
+        <v>44564</v>
       </c>
       <c r="B2">
-        <v>23</v>
+        <v>24.5</v>
       </c>
       <c r="C2">
-        <v>21</v>
+        <v>25.01</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>44563</v>
+        <v>44565</v>
       </c>
       <c r="B3">
-        <v>24</v>
+        <v>25.49</v>
       </c>
       <c r="C3">
-        <v>22</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>44564</v>
+        <v>44566</v>
       </c>
       <c r="B4">
-        <v>25</v>
+        <v>29.12</v>
       </c>
       <c r="C4">
-        <v>23</v>
+        <v>28.73</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>44565</v>
+        <v>44567</v>
       </c>
       <c r="B5">
-        <v>26</v>
+        <v>27.16</v>
       </c>
       <c r="C5">
-        <v>24</v>
+        <v>28.24</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>44566</v>
+        <v>44568</v>
       </c>
       <c r="B6">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6">
-        <v>25</v>
+        <v>24.69</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>44567</v>
+        <v>44569</v>
       </c>
       <c r="B7">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C7">
-        <v>26</v>
+        <v>26.08</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>44568</v>
+        <v>44571</v>
       </c>
       <c r="B8">
-        <v>29</v>
+        <v>26.96</v>
       </c>
       <c r="C8">
-        <v>27</v>
+        <v>26.86</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>44569</v>
+        <v>44572</v>
       </c>
       <c r="B9">
-        <v>30</v>
+        <v>29.22</v>
       </c>
       <c r="C9">
-        <v>28</v>
+        <v>28.73</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>44570</v>
+        <v>44573</v>
       </c>
       <c r="B10">
-        <v>31</v>
+        <v>23.14</v>
       </c>
       <c r="C10">
-        <v>29</v>
+        <v>22.11</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>44571</v>
+        <v>44574</v>
       </c>
       <c r="B11">
-        <v>32</v>
+        <v>23.73</v>
       </c>
       <c r="C11">
-        <v>30</v>
+        <v>23.82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>44575</v>
+      </c>
+      <c r="B12">
+        <v>21.67</v>
+      </c>
+      <c r="C12">
+        <v>21.76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>44590</v>
+      </c>
+      <c r="B13">
+        <v>27.84</v>
+      </c>
+      <c r="C13">
+        <v>27.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>44591</v>
+      </c>
+      <c r="B14">
+        <v>26.5</v>
+      </c>
+      <c r="C14">
+        <v>25.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>44592</v>
+      </c>
+      <c r="B15">
+        <v>28.73</v>
+      </c>
+      <c r="C15">
+        <v>28.53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B16">
+        <v>22.4</v>
+      </c>
+      <c r="C16">
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>44594</v>
+      </c>
+      <c r="B17">
+        <v>26.18</v>
+      </c>
+      <c r="C17">
+        <v>26.57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>44595</v>
+      </c>
+      <c r="B18">
+        <v>25.7</v>
+      </c>
+      <c r="C18">
+        <v>24.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>44596</v>
+      </c>
+      <c r="B19">
+        <v>26.37</v>
+      </c>
+      <c r="C19">
+        <v>26.86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>44601</v>
+      </c>
+      <c r="B20">
+        <v>26.47</v>
+      </c>
+      <c r="C20">
+        <v>26.67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>44602</v>
+      </c>
+      <c r="B21">
+        <v>27.64</v>
+      </c>
+      <c r="C21">
+        <v>28.04</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>44603</v>
+      </c>
+      <c r="B22">
+        <v>28.55</v>
+      </c>
+      <c r="C22">
+        <v>29.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>44604</v>
+      </c>
+      <c r="B23">
+        <v>29.56</v>
+      </c>
+      <c r="C23">
+        <v>20.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>44606</v>
+      </c>
+      <c r="B24">
+        <v>28.14</v>
+      </c>
+      <c r="C24">
+        <v>28.92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>44607</v>
+      </c>
+      <c r="B25">
+        <v>27.83</v>
+      </c>
+      <c r="C25">
+        <v>28.84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>44609</v>
+      </c>
+      <c r="B26">
+        <v>22.8</v>
+      </c>
+      <c r="C26">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>44610</v>
+      </c>
+      <c r="B27">
+        <v>23.86</v>
+      </c>
+      <c r="C27">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>44611</v>
+      </c>
+      <c r="B28">
+        <v>23.22</v>
+      </c>
+      <c r="C28">
+        <v>23.39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>44613</v>
+      </c>
+      <c r="B29">
+        <v>24.9</v>
+      </c>
+      <c r="C29">
+        <v>24.31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>44614</v>
+      </c>
+      <c r="B30">
+        <v>31.27</v>
+      </c>
+      <c r="C30">
+        <v>31.47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>44615</v>
+      </c>
+      <c r="B31">
+        <v>27.16</v>
+      </c>
+      <c r="C31">
+        <v>28.57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>44616</v>
+      </c>
+      <c r="B32">
+        <v>29.05</v>
+      </c>
+      <c r="C32">
+        <v>29.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>44617</v>
+      </c>
+      <c r="B33">
+        <v>20.38</v>
+      </c>
+      <c r="C33">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>44618</v>
+      </c>
+      <c r="B34">
+        <v>27.02</v>
+      </c>
+      <c r="C34">
+        <v>28.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B35">
+        <v>28.04</v>
+      </c>
+      <c r="C35">
+        <v>27.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>44622</v>
+      </c>
+      <c r="B36">
+        <v>26.47</v>
+      </c>
+      <c r="C36">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>44623</v>
+      </c>
+      <c r="B37">
+        <v>27.18</v>
+      </c>
+      <c r="C37">
+        <v>27.08</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>44624</v>
+      </c>
+      <c r="B38">
+        <v>22.04</v>
+      </c>
+      <c r="C38">
+        <v>22.53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>44625</v>
+      </c>
+      <c r="B39">
+        <v>25.88</v>
+      </c>
+      <c r="C39">
+        <v>25.88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>44626</v>
+      </c>
+      <c r="B40">
+        <v>32.08</v>
+      </c>
+      <c r="C40">
+        <v>31.37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>44627</v>
+      </c>
+      <c r="B41">
+        <v>24.5</v>
+      </c>
+      <c r="C41">
+        <v>25.3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>